<commit_message>
Finished updating Analysis 0 and 1
</commit_message>
<xml_diff>
--- a/Data/Raw/Population 2020-2024.xlsx
+++ b/Data/Raw/Population 2020-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prisha/Desktop/Final Project EDE/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA36D552-E665-9243-A98D-BD7EE41C1F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA84204D-7AAF-0C44-96C5-A342E27E3E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST-EST2024-POP" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
     <t>Hawaii</t>
   </si>
   <si>
-    <t>States</t>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -1523,6 +1523,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010078B597BA3CDC584DBB389A397F0D357D" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="def0205ca3926f58531bbff327d3b7d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f0a2a16-30d7-495a-94e9-8ccd05e9ff7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4ac9f1c406f38ef80a11d9afb7a8526" ns2:_="">
     <xsd:import namespace="7f0a2a16-30d7-495a-94e9-8ccd05e9ff7a"/>
@@ -1660,22 +1675,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B017866-70C9-4037-81EF-1573C0F8DFD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAB57E6D-D769-4AAB-B8C3-458A53660BA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BB229F4-89E9-4E55-9B28-FC8DD5EFA258}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1691,21 +1708,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAB57E6D-D769-4AAB-B8C3-458A53660BA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B017866-70C9-4037-81EF-1573C0F8DFD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added all analyses, only written inferences are left
</commit_message>
<xml_diff>
--- a/Data/Raw/Population 2020-2024.xlsx
+++ b/Data/Raw/Population 2020-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prisha/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prisha/Desktop/Final Project EDE/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4808D08-3B3E-0941-84C0-F6DA3390B3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6416B1F5-AE4A-E641-8D87-59CBB5558C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST-EST2024-POP" sheetId="1" r:id="rId1"/>
@@ -43,670 +43,160 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alabama</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alaska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arizona</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arkansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>California</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Colorado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Connecticut</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Delaware</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>District of Columbia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Florida</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Georgia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Hawaii</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Idaho</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Illinois</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Indiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Iowa</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kentucky</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Louisiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maine</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maryland</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Massachusetts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Michigan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Minnesota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Mississippi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Missouri</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Montana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nebraska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nevada</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Hampshire</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Jersey</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Mexico</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New York</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Ohio</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oklahoma</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oregon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Pennsylvania</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Rhode Island</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Tennessee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Texas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Utah</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Vermont</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Washington</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>West Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wisconsin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wyoming</t>
-    </r>
-  </si>
-  <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
   </si>
 </sst>
 </file>
@@ -731,11 +221,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="9"/>
-      <name val="MS sans serif"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="MS sans serif"/>
     </font>
@@ -744,6 +229,11 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="MS sans serif"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -814,24 +304,22 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,7 +628,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1151,25 +639,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="6">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
         <v>2020</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="5">
         <v>2021</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="5">
         <v>2022</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="5">
         <v>2023</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="16" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
+      <c r="A2" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>5033094</v>
@@ -1184,9 +672,9 @@
         <v>5117673</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B3" s="3">
         <v>733017</v>
@@ -1201,8 +689,8 @@
         <v>736510</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -1218,8 +706,8 @@
         <v>7473027</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3">
@@ -1235,8 +723,8 @@
         <v>3069463</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
@@ -1252,8 +740,8 @@
         <v>39198693</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3">
@@ -1269,8 +757,8 @@
         <v>5901339</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3">
@@ -1286,8 +774,8 @@
         <v>3643023</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3">
@@ -1303,8 +791,8 @@
         <v>1036423</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3">
@@ -1320,8 +808,8 @@
         <v>687324</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
@@ -1337,8 +825,8 @@
         <v>22904868</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3">
@@ -1354,9 +842,9 @@
         <v>11064432</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
+    <row r="13" spans="1:5" ht="16">
+      <c r="A13" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="B13" s="3">
         <v>1451252</v>
@@ -1371,9 +859,9 @@
         <v>1441387</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4" t="s">
-        <v>12</v>
+    <row r="14" spans="1:5" ht="16">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="3">
         <v>1849415</v>
@@ -1388,9 +876,9 @@
         <v>1971122</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
-        <v>13</v>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="B15" s="3">
         <v>12799088</v>
@@ -1405,9 +893,9 @@
         <v>12642259</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>6790497</v>
@@ -1422,9 +910,9 @@
         <v>6880131</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>3191141</v>
@@ -1439,9 +927,9 @@
         <v>3218414</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>2938172</v>
@@ -1456,9 +944,9 @@
         <v>2951500</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B19" s="3">
         <v>4508318</v>
@@ -1473,9 +961,9 @@
         <v>4550595</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B20" s="3">
         <v>4652301</v>
@@ -1490,9 +978,9 @@
         <v>4588071</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4" t="s">
-        <v>19</v>
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B21" s="3">
         <v>1364571</v>
@@ -1507,9 +995,9 @@
         <v>1399646</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4" t="s">
-        <v>20</v>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B22" s="3">
         <v>6177935</v>
@@ -1524,9 +1012,9 @@
         <v>6217062</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>21</v>
+    <row r="23" spans="1:5" ht="16">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B23" s="3">
         <v>6994598</v>
@@ -1541,9 +1029,9 @@
         <v>7066568</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4" t="s">
-        <v>22</v>
+    <row r="24" spans="1:5" ht="16">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B24" s="3">
         <v>10072703</v>
@@ -1558,9 +1046,9 @@
         <v>10083356</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4" t="s">
-        <v>23</v>
+    <row r="25" spans="1:5" ht="16">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B25" s="3">
         <v>5710735</v>
@@ -1575,9 +1063,9 @@
         <v>5753048</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
-        <v>24</v>
+    <row r="26" spans="1:5" ht="16">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="3">
         <v>2958536</v>
@@ -1592,9 +1080,9 @@
         <v>2943172</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4" t="s">
-        <v>25</v>
+    <row r="27" spans="1:5" ht="16">
+      <c r="A27" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B27" s="3">
         <v>6154744</v>
@@ -1609,9 +1097,9 @@
         <v>6208038</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4" t="s">
-        <v>26</v>
+    <row r="28" spans="1:5" ht="16">
+      <c r="A28" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="B28" s="3">
         <v>1087230</v>
@@ -1626,9 +1114,9 @@
         <v>1131302</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4" t="s">
-        <v>27</v>
+    <row r="29" spans="1:5" ht="16">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B29" s="3">
         <v>1963387</v>
@@ -1643,9 +1131,9 @@
         <v>1987864</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4" t="s">
-        <v>28</v>
+    <row r="30" spans="1:5" ht="16">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="3">
         <v>3116967</v>
@@ -1660,9 +1148,9 @@
         <v>3214363</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="4" t="s">
-        <v>29</v>
+    <row r="31" spans="1:5" ht="16">
+      <c r="A31" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B31" s="3">
         <v>1378756</v>
@@ -1677,9 +1165,9 @@
         <v>1402199</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="4" t="s">
-        <v>30</v>
+    <row r="32" spans="1:5" ht="16">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B32" s="3">
         <v>9272794</v>
@@ -1694,9 +1182,9 @@
         <v>9379642</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="4" t="s">
-        <v>31</v>
+    <row r="33" spans="1:5" ht="16">
+      <c r="A33" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="3">
         <v>2118606</v>
@@ -1711,9 +1199,9 @@
         <v>2121164</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="4" t="s">
-        <v>32</v>
+    <row r="34" spans="1:5" ht="16">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B34" s="3">
         <v>20105171</v>
@@ -1728,9 +1216,9 @@
         <v>19737367</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="4" t="s">
-        <v>33</v>
+    <row r="35" spans="1:5" ht="16">
+      <c r="A35" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B35" s="3">
         <v>10449652</v>
@@ -1745,9 +1233,9 @@
         <v>10881189</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="4" t="s">
-        <v>34</v>
+    <row r="36" spans="1:5" ht="16">
+      <c r="A36" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B36" s="3">
         <v>779563</v>
@@ -1762,9 +1250,9 @@
         <v>789047</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4" t="s">
-        <v>35</v>
+    <row r="37" spans="1:5" ht="16">
+      <c r="A37" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B37" s="3">
         <v>11798905</v>
@@ -1779,9 +1267,9 @@
         <v>11824034</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="4" t="s">
-        <v>36</v>
+    <row r="38" spans="1:5" ht="16">
+      <c r="A38" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="B38" s="3">
         <v>3965415</v>
@@ -1796,9 +1284,9 @@
         <v>4063882</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="4" t="s">
-        <v>37</v>
+    <row r="39" spans="1:5" ht="16">
+      <c r="A39" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B39" s="3">
         <v>4243779</v>
@@ -1813,9 +1301,9 @@
         <v>4253653</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4" t="s">
-        <v>38</v>
+    <row r="40" spans="1:5" ht="16">
+      <c r="A40" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="B40" s="3">
         <v>12996143</v>
@@ -1830,9 +1318,9 @@
         <v>13017721</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="4" t="s">
-        <v>39</v>
+    <row r="41" spans="1:5" ht="16">
+      <c r="A41" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B41" s="3">
         <v>1096530</v>
@@ -1847,9 +1335,9 @@
         <v>1103429</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4" t="s">
-        <v>40</v>
+    <row r="42" spans="1:5" ht="16">
+      <c r="A42" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="B42" s="3">
         <v>5132249</v>
@@ -1864,9 +1352,9 @@
         <v>5387830</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4" t="s">
-        <v>41</v>
+    <row r="43" spans="1:5" ht="16">
+      <c r="A43" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B43" s="3">
         <v>887948</v>
@@ -1881,9 +1369,9 @@
         <v>918305</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="4" t="s">
-        <v>42</v>
+    <row r="44" spans="1:5" ht="16">
+      <c r="A44" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B44" s="3">
         <v>6927904</v>
@@ -1898,9 +1386,9 @@
         <v>7148304</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="4" t="s">
-        <v>43</v>
+    <row r="45" spans="1:5" ht="16">
+      <c r="A45" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="B45" s="3">
         <v>29239570</v>
@@ -1915,9 +1403,9 @@
         <v>30727890</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="4" t="s">
-        <v>44</v>
+    <row r="46" spans="1:5" ht="16">
+      <c r="A46" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B46" s="3">
         <v>3284077</v>
@@ -1932,9 +1420,9 @@
         <v>3443222</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="4" t="s">
-        <v>45</v>
+    <row r="47" spans="1:5" ht="16">
+      <c r="A47" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="B47" s="3">
         <v>642977</v>
@@ -1949,9 +1437,9 @@
         <v>648708</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="4" t="s">
-        <v>46</v>
+    <row r="48" spans="1:5" ht="16">
+      <c r="A48" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B48" s="3">
         <v>8637615</v>
@@ -1966,9 +1454,9 @@
         <v>8734685</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="4" t="s">
-        <v>47</v>
+    <row r="49" spans="1:6" ht="16">
+      <c r="A49" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B49" s="3">
         <v>7727209</v>
@@ -1983,9 +1471,9 @@
         <v>7857320</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="4" t="s">
-        <v>48</v>
+    <row r="50" spans="1:6" ht="16">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B50" s="3">
         <v>1791646</v>
@@ -2000,9 +1488,9 @@
         <v>1770495</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="4" t="s">
-        <v>49</v>
+    <row r="51" spans="1:6" ht="16">
+      <c r="A51" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B51" s="3">
         <v>5897375</v>
@@ -2017,9 +1505,9 @@
         <v>5930405</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="4" t="s">
-        <v>50</v>
+    <row r="52" spans="1:6" ht="16">
+      <c r="A52" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B52" s="3">
         <v>577681</v>
@@ -2042,7 +1530,7 @@
       <c r="E54"/>
       <c r="F54"/>
     </row>
-    <row r="55" spans="1:6" s="5" customFormat="1">
+    <row r="55" spans="1:6" s="4" customFormat="1">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -2130,6 +1618,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010078B597BA3CDC584DBB389A397F0D357D" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="def0205ca3926f58531bbff327d3b7d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f0a2a16-30d7-495a-94e9-8ccd05e9ff7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4ac9f1c406f38ef80a11d9afb7a8526" ns2:_="">
     <xsd:import namespace="7f0a2a16-30d7-495a-94e9-8ccd05e9ff7a"/>
@@ -2267,15 +1764,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2283,6 +1771,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAB57E6D-D769-4AAB-B8C3-458A53660BA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BB229F4-89E9-4E55-9B28-FC8DD5EFA258}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2300,14 +1796,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAB57E6D-D769-4AAB-B8C3-458A53660BA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B017866-70C9-4037-81EF-1573C0F8DFD6}">
   <ds:schemaRefs>

</xml_diff>